<commit_message>
[spreadsheet] big rewrite of J::Spreadsheet
 This arose out of a need for data type annotations.  I've rewritten
 J::Spreadsheet to extract the type annotations directly out of the
 spreadsheet, instead of relying upon SQLT::Parser::Spreadsheet to do
 that. SQLT::P::S  wasn't really doing anything useful for us, so it
 made sense to move it's critical functionality into J::S, and let
 ::Result::Dataset query the J::S object directly for the type annotations.

 Before, bugs in SQLT::P::S caused everything to accidentally be saved as
 varchars in the datastore.  Now we save things as text fields, but do
 sorting in DatasetData and data.cgi if we have numeric data.  We also save
 type info when we create ::R::DatasetColumns.

 Really, Standalone.pm, data.cgi, and standalone-app.t should be in a
 different commit.

 Also, update basic.xlsx to make it consistent with basic.xls.
</commit_message>
<xml_diff>
--- a/t/etc/data/basic.xlsx
+++ b/t/etc/data/basic.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="60" windowWidth="25000" windowHeight="17300" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dog Roster" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="110304" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:ArchID Flags="0"/>
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -57,9 +57,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -414,12 +418,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
@@ -490,9 +491,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -503,16 +503,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -523,16 +520,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>